<commit_message>
done with base functional
</commit_message>
<xml_diff>
--- a/test_data/login_data.xlsx
+++ b/test_data/login_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\auto_selenium_test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFEFDEB-844D-45D4-A454-ED7E3DA5B7B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1527034-B943-488E-94B6-B6E6D11E7F02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -383,7 +383,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,7 +432,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>